<commit_message>
New data pull from 2023-05 and reran analysis.
</commit_message>
<xml_diff>
--- a/analysis/years.xlsx
+++ b/analysis/years.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="years" sheetId="1" r:id="rId1"/>
     <sheet name="decay" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -592,15 +592,52 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Most Supplemental Data Links</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> are Recent</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.9791557305336837E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -635,177 +672,11 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>years!$A$2:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>years!$C$2:$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>293</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>740</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>386</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-77E1-498E-9744-C7529CEE6322}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -816,132 +687,215 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>years!$A$2:$A$23</c:f>
+              <c:f>years!$A$101:$A$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>years!$D$2:$D$23</c:f>
+              <c:f>years!$C$101:$C$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>293</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-77E1-498E-9744-C7529CEE6322}"/>
+              <c16:uniqueId val="{00000000-6467-45EE-8B0F-CE94B5D92C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -953,13 +907,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="50"/>
-        <c:overlap val="100"/>
-        <c:axId val="555729176"/>
-        <c:axId val="555729504"/>
+        <c:gapWidth val="0"/>
+        <c:overlap val="-27"/>
+        <c:axId val="497485104"/>
+        <c:axId val="497495928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="555729176"/>
+        <c:axId val="497485104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555729504"/>
+        <c:crossAx val="497495928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,9 +964,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555729504"/>
+        <c:axId val="497495928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="800"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1061,9 +1016,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555729176"/>
+        <c:crossAx val="497485104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="800"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1073,38 +1029,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1157,7 +1081,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1453,42 +1376,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1533,7 +1422,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1737,23 +1626,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1858,8 +1746,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1991,20 +1879,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2557,20 +2444,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>384810</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2888,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E23"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2916,639 +2803,482 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2022</v>
+        <v>1894</v>
       </c>
       <c r="B2">
-        <v>2779</v>
-      </c>
-      <c r="C2">
-        <v>293</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <f>D2/C2</f>
-        <v>3.0716723549488054E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2021</v>
+        <v>1895</v>
       </c>
       <c r="B3">
-        <v>7919</v>
-      </c>
-      <c r="C3">
-        <v>740</v>
-      </c>
-      <c r="D3">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E22" si="0">D3/C3</f>
-        <v>2.1621621621621623E-2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2020</v>
+        <v>1897</v>
       </c>
       <c r="B4">
-        <v>7496</v>
-      </c>
-      <c r="C4">
-        <v>386</v>
-      </c>
-      <c r="D4">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>3.367875647668394E-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2019</v>
+        <v>1904</v>
       </c>
       <c r="B5">
-        <v>6699</v>
-      </c>
-      <c r="C5">
-        <v>115</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>4.3478260869565216E-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2018</v>
+        <v>1905</v>
       </c>
       <c r="B6">
-        <v>7423</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2017</v>
+        <v>1906</v>
       </c>
       <c r="B7">
-        <v>8936</v>
-      </c>
-      <c r="C7">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2016</v>
+        <v>1908</v>
       </c>
       <c r="B8">
-        <v>9021</v>
-      </c>
-      <c r="C8">
-        <v>57</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.14035087719298245</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2015</v>
+        <v>1909</v>
       </c>
       <c r="B9">
-        <v>8965</v>
-      </c>
-      <c r="C9">
-        <v>53</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>7.5471698113207544E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2014</v>
+        <v>1910</v>
       </c>
       <c r="B10">
-        <v>9047</v>
-      </c>
-      <c r="C10">
-        <v>43</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>2.3255813953488372E-2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2013</v>
+        <v>1911</v>
       </c>
       <c r="B11">
-        <v>8136</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2012</v>
+        <v>1912</v>
       </c>
       <c r="B12">
-        <v>7667</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2011</v>
+        <v>1913</v>
       </c>
       <c r="B13">
-        <v>6761</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2010</v>
+        <v>1914</v>
       </c>
       <c r="B14">
-        <v>6516</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2009</v>
+        <v>1915</v>
       </c>
       <c r="B15">
-        <v>6102</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2008</v>
+        <v>1916</v>
       </c>
       <c r="B16">
-        <v>5111</v>
-      </c>
-      <c r="C16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1917</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1918</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1919</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1920</v>
+      </c>
+      <c r="B20">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2007</v>
-      </c>
-      <c r="B17">
-        <v>4781</v>
-      </c>
-      <c r="C17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2006</v>
-      </c>
-      <c r="B18">
-        <v>4453</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2005</v>
-      </c>
-      <c r="B19">
-        <v>3480</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>2004</v>
-      </c>
-      <c r="B20">
-        <v>3512</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2003</v>
+        <v>1921</v>
       </c>
       <c r="B21">
-        <v>3167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2002</v>
+        <v>1922</v>
       </c>
       <c r="B22">
-        <v>2951</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2001</v>
+        <v>1923</v>
       </c>
       <c r="B23">
-        <v>2861</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2000</v>
+        <v>1924</v>
       </c>
       <c r="B24">
-        <v>2693</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>1999</v>
+        <v>1925</v>
       </c>
       <c r="B25">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>1998</v>
+        <v>1926</v>
       </c>
       <c r="B26">
-        <v>2340</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>1997</v>
+        <v>1927</v>
       </c>
       <c r="B27">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>1996</v>
+        <v>1928</v>
       </c>
       <c r="B28">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>1995</v>
+        <v>1929</v>
       </c>
       <c r="B29">
-        <v>1868</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>1994</v>
+        <v>1930</v>
       </c>
       <c r="B30">
-        <v>1799</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>1993</v>
+        <v>1931</v>
       </c>
       <c r="B31">
-        <v>1704</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>1992</v>
+        <v>1932</v>
       </c>
       <c r="B32">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>1991</v>
+        <v>1933</v>
       </c>
       <c r="B33">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>1990</v>
+        <v>1934</v>
       </c>
       <c r="B34">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>1989</v>
+        <v>1935</v>
       </c>
       <c r="B35">
-        <v>1362</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>1988</v>
+        <v>1936</v>
       </c>
       <c r="B36">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>1987</v>
+        <v>1937</v>
       </c>
       <c r="B37">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>1986</v>
+        <v>1938</v>
       </c>
       <c r="B38">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>1985</v>
+        <v>1939</v>
       </c>
       <c r="B39">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>1984</v>
+        <v>1940</v>
       </c>
       <c r="B40">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1983</v>
+        <v>1941</v>
       </c>
       <c r="B41">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>1982</v>
+        <v>1942</v>
       </c>
       <c r="B42">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>1981</v>
+        <v>1943</v>
       </c>
       <c r="B43">
-        <v>973</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>1980</v>
+        <v>1944</v>
       </c>
       <c r="B44">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>1979</v>
+        <v>1945</v>
       </c>
       <c r="B45">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1978</v>
+        <v>1946</v>
       </c>
       <c r="B46">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1977</v>
+        <v>1947</v>
       </c>
       <c r="B47">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1976</v>
+        <v>1948</v>
       </c>
       <c r="B48">
-        <v>689</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>1975</v>
+        <v>1949</v>
       </c>
       <c r="B49">
-        <v>683</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>1974</v>
+        <v>1950</v>
       </c>
       <c r="B50">
-        <v>582</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>1973</v>
+        <v>1951</v>
       </c>
       <c r="B51">
-        <v>560</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>1972</v>
+        <v>1952</v>
       </c>
       <c r="B52">
-        <v>500</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>1971</v>
+        <v>1953</v>
       </c>
       <c r="B53">
-        <v>478</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>1970</v>
+        <v>1954</v>
       </c>
       <c r="B54">
-        <v>512</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>1969</v>
+        <v>1955</v>
       </c>
       <c r="B55">
-        <v>486</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>1968</v>
+        <v>1956</v>
       </c>
       <c r="B56">
-        <v>435</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>1967</v>
+        <v>1957</v>
       </c>
       <c r="B57">
-        <v>413</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>1966</v>
+        <v>1958</v>
       </c>
       <c r="B58">
-        <v>387</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>1965</v>
+        <v>1959</v>
       </c>
       <c r="B59">
-        <v>351</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>1964</v>
+        <v>1960</v>
       </c>
       <c r="B60">
-        <v>339</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="B61">
-        <v>318</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -3561,485 +3291,642 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>1961</v>
+        <v>1963</v>
       </c>
       <c r="B63">
-        <v>262</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>1960</v>
+        <v>1964</v>
       </c>
       <c r="B64">
-        <v>271</v>
+        <v>339</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>1959</v>
+        <v>1965</v>
       </c>
       <c r="B65">
-        <v>179</v>
+        <v>351</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>1958</v>
+        <v>1966</v>
       </c>
       <c r="B66">
-        <v>155</v>
+        <v>387</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>1957</v>
+        <v>1967</v>
       </c>
       <c r="B67">
-        <v>149</v>
+        <v>413</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>1956</v>
+        <v>1968</v>
       </c>
       <c r="B68">
-        <v>142</v>
+        <v>435</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>1955</v>
+        <v>1969</v>
       </c>
       <c r="B69">
-        <v>149</v>
+        <v>486</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>1954</v>
+        <v>1970</v>
       </c>
       <c r="B70">
-        <v>149</v>
+        <v>512</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>1953</v>
+        <v>1971</v>
       </c>
       <c r="B71">
-        <v>150</v>
+        <v>478</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>1952</v>
+        <v>1972</v>
       </c>
       <c r="B72">
-        <v>173</v>
+        <v>500</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>1951</v>
+        <v>1973</v>
       </c>
       <c r="B73">
-        <v>169</v>
+        <v>560</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>1950</v>
+        <v>1974</v>
       </c>
       <c r="B74">
-        <v>149</v>
+        <v>582</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>1949</v>
+        <v>1975</v>
       </c>
       <c r="B75">
-        <v>143</v>
+        <v>683</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>1948</v>
+        <v>1976</v>
       </c>
       <c r="B76">
-        <v>150</v>
+        <v>689</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>1947</v>
+        <v>1977</v>
       </c>
       <c r="B77">
-        <v>75</v>
+        <v>805</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>1946</v>
+        <v>1978</v>
       </c>
       <c r="B78">
-        <v>74</v>
+        <v>802</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>1945</v>
+        <v>1979</v>
       </c>
       <c r="B79">
-        <v>46</v>
+        <v>811</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>1944</v>
+        <v>1980</v>
       </c>
       <c r="B80">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>1943</v>
+        <v>1981</v>
       </c>
       <c r="B81">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>973</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>1942</v>
+        <v>1982</v>
       </c>
       <c r="B82">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>1941</v>
+        <v>1983</v>
       </c>
       <c r="B83">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>1940</v>
+        <v>1984</v>
       </c>
       <c r="B84">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>1939</v>
+        <v>1985</v>
       </c>
       <c r="B85">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>1938</v>
+        <v>1986</v>
       </c>
       <c r="B86">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>1937</v>
+        <v>1987</v>
       </c>
       <c r="B87">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>1936</v>
+        <v>1988</v>
       </c>
       <c r="B88">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>1935</v>
+        <v>1989</v>
       </c>
       <c r="B89">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>1934</v>
+        <v>1990</v>
       </c>
       <c r="B90">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>1933</v>
+        <v>1991</v>
       </c>
       <c r="B91">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>1932</v>
+        <v>1992</v>
       </c>
       <c r="B92">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>1931</v>
+        <v>1993</v>
       </c>
       <c r="B93">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>1930</v>
+        <v>1994</v>
       </c>
       <c r="B94">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>1929</v>
+        <v>1995</v>
       </c>
       <c r="B95">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>1928</v>
+        <v>1996</v>
       </c>
       <c r="B96">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>1927</v>
+        <v>1997</v>
       </c>
       <c r="B97">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>1926</v>
+        <v>1998</v>
       </c>
       <c r="B98">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>1925</v>
+        <v>1999</v>
       </c>
       <c r="B99">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>1924</v>
+        <v>2000</v>
       </c>
       <c r="B100">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>1923</v>
+        <v>2001</v>
       </c>
       <c r="B101">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2861</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>1922</v>
+        <v>2002</v>
       </c>
       <c r="B102">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2951</v>
+      </c>
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" s="1">
+        <f>D102/C102</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>1921</v>
+        <v>2003</v>
       </c>
       <c r="B103">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>1920</v>
+        <v>2004</v>
       </c>
       <c r="B104">
+        <v>3512</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1">
+        <f>D104/C104</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>2005</v>
+      </c>
+      <c r="B105">
+        <v>3480</v>
+      </c>
+      <c r="C105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>2006</v>
+      </c>
+      <c r="B106">
+        <v>4453</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>2007</v>
+      </c>
+      <c r="B107">
+        <v>4781</v>
+      </c>
+      <c r="C107">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>2008</v>
+      </c>
+      <c r="B108">
+        <v>5111</v>
+      </c>
+      <c r="C108">
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <v>1919</v>
-      </c>
-      <c r="B105">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <v>1918</v>
-      </c>
-      <c r="B106">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>2009</v>
+      </c>
+      <c r="B109">
+        <v>6102</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>2010</v>
+      </c>
+      <c r="B110">
+        <v>6516</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" s="1">
+        <f>D110/C110</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>2011</v>
+      </c>
+      <c r="B111">
+        <v>6761</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>2012</v>
+      </c>
+      <c r="B112">
+        <v>7667</v>
+      </c>
+      <c r="C112">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>2013</v>
+      </c>
+      <c r="B113">
+        <v>8136</v>
+      </c>
+      <c r="C113">
+        <v>5</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+      <c r="E113" s="1">
+        <f t="shared" ref="E113:E122" si="0">D113/C113</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>2014</v>
+      </c>
+      <c r="B114">
+        <v>9047</v>
+      </c>
+      <c r="C114">
+        <v>43</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>2015</v>
+      </c>
+      <c r="B115">
+        <v>8965</v>
+      </c>
+      <c r="C115">
+        <v>53</v>
+      </c>
+      <c r="D115">
+        <v>4</v>
+      </c>
+      <c r="E115" s="1">
+        <f t="shared" si="0"/>
+        <v>7.5471698113207544E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>2016</v>
+      </c>
+      <c r="B116">
+        <v>9021</v>
+      </c>
+      <c r="C116">
+        <v>57</v>
+      </c>
+      <c r="D116">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <v>1917</v>
-      </c>
-      <c r="B107">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <v>1916</v>
-      </c>
-      <c r="B108">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <v>1915</v>
-      </c>
-      <c r="B109">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>1914</v>
-      </c>
-      <c r="B110">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <v>1913</v>
-      </c>
-      <c r="B111">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <v>1912</v>
-      </c>
-      <c r="B112">
+      <c r="E116" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14035087719298245</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>2017</v>
+      </c>
+      <c r="B117">
+        <v>8936</v>
+      </c>
+      <c r="C117">
+        <v>24</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="E117" s="1">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>2018</v>
+      </c>
+      <c r="B118">
+        <v>7423</v>
+      </c>
+      <c r="C118">
+        <v>50</v>
+      </c>
+      <c r="D118">
+        <v>4</v>
+      </c>
+      <c r="E118" s="1">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2019</v>
+      </c>
+      <c r="B119">
+        <v>6699</v>
+      </c>
+      <c r="C119">
+        <v>115</v>
+      </c>
+      <c r="D119">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <v>1911</v>
-      </c>
-      <c r="B113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <v>1910</v>
-      </c>
-      <c r="B114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <v>1909</v>
-      </c>
-      <c r="B115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <v>1908</v>
-      </c>
-      <c r="B116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <v>1906</v>
-      </c>
-      <c r="B117">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <v>1905</v>
-      </c>
-      <c r="B118">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <v>1904</v>
-      </c>
-      <c r="B119">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E119" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>1897</v>
+        <v>2020</v>
       </c>
       <c r="B120">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7496</v>
+      </c>
+      <c r="C120">
+        <v>386</v>
+      </c>
+      <c r="D120">
+        <v>13</v>
+      </c>
+      <c r="E120" s="1">
+        <f t="shared" si="0"/>
+        <v>3.367875647668394E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>1895</v>
+        <v>2021</v>
       </c>
       <c r="B121">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7919</v>
+      </c>
+      <c r="C121">
+        <v>740</v>
+      </c>
+      <c r="D121">
+        <v>16</v>
+      </c>
+      <c r="E121" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1621621621621623E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>1894</v>
+        <v>2022</v>
       </c>
       <c r="B122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2779</v>
+      </c>
+      <c r="C122">
+        <v>293</v>
+      </c>
+      <c r="D122">
+        <v>9</v>
+      </c>
+      <c r="E122" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0716723549488054E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -4048,8 +3935,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="D3:F15">
-    <sortCondition descending="1" ref="D3:D15"/>
+  <sortState ref="A2:E123">
+    <sortCondition ref="A2:A123"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4061,7 +3948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>